<commit_message>
them co so du lieu
</commit_message>
<xml_diff>
--- a/TESTCASE_OF_HETHONGBANVE.xlsx
+++ b/TESTCASE_OF_HETHONGBANVE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huqedgar_user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FCC44C-C600-4472-990A-CB0193403D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE639AF-D0CE-48FE-B489-E8858ED9BD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="385">
   <si>
     <t>STT</t>
   </si>
@@ -1083,9 +1083,6 @@
     <t>Thời gian bắt đầu và thời gian kết thúc được thay đổi
 cập nhật đến ngày hiện tại của hệ thống 
 (giờ chuyến đi vẫn giữ nguyên)</t>
-  </si>
-  <si>
-    <t>Nhập vào textfield tìm kiếm: An Giang</t>
   </si>
   <si>
     <t>Nhập vào textfield tìm kiếm: Hà Nội</t>
@@ -1213,9 +1210,6 @@
     <t>Nhập vào textfield tìm kiếm xe theo tên: Hyundai Solati</t>
   </si>
   <si>
-    <t>Tableview chuyến đi hiển thị thông tin chuyến đi mà tên chuyến có từ "An Giang"</t>
-  </si>
-  <si>
     <t>Nhập vào textfield tìm kiếm xe theo mã chuyến đi: 21</t>
   </si>
   <si>
@@ -1523,6 +1517,26 @@
 B4. Nhập trạng thái: 0
 B5. Nhập mã chuyến: 10
 B6. Ấn chọn nút "Sửa"</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập thành công
+2. Đặt vé cho xe có mã: 25
+3. Vào được chức năng quản trị
+4. Nhập đủ thông tin</t>
+  </si>
+  <si>
+    <t>B1. Nhập mã xe: 24
+B2. Nhập tên xe: Toyota Hiace (2022)
+B3. Nhập biển số: 51H-123.45
+B4. Nhập trạng thái: 0
+B5. Nhập mã chuyến: 5
+B6. Ấn chọn nút "Sửa"</t>
+  </si>
+  <si>
+    <t>Tableview chuyến đi hiển thị thông tin chuyến đi mà tên chuyến có từ "Bình Dương"</t>
+  </si>
+  <si>
+    <t>Nhập vào textfield tìm kiếm: Bình Dương</t>
   </si>
 </sst>
 </file>
@@ -1988,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H76" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="D122" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
@@ -4084,7 +4098,7 @@
         <v>37</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G67" s="9" t="s">
         <v>101</v>
@@ -4116,7 +4130,7 @@
         <v>37</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>176</v>
@@ -4148,7 +4162,7 @@
         <v>37</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>183</v>
@@ -4180,7 +4194,7 @@
         <v>37</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G70" s="9" t="s">
         <v>186</v>
@@ -4212,13 +4226,13 @@
         <v>37</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>190</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I71" s="8"/>
       <c r="J71" s="15" t="s">
@@ -4244,7 +4258,7 @@
         <v>37</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>192</v>
@@ -4276,13 +4290,13 @@
         <v>37</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>195</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I73" s="8"/>
       <c r="J73" s="15" t="s">
@@ -4308,7 +4322,7 @@
         <v>37</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>101</v>
@@ -4348,7 +4362,7 @@
         <v>200</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I75" s="17"/>
       <c r="J75" s="15" t="s">
@@ -4371,7 +4385,7 @@
         <v>198</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>199</v>
@@ -4380,7 +4394,7 @@
         <v>200</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
@@ -4403,7 +4417,7 @@
         <v>203</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>204</v>
@@ -4435,7 +4449,7 @@
         <v>206</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F78" s="10" t="s">
         <v>204</v>
@@ -4467,13 +4481,13 @@
         <v>207</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H79" s="8" t="s">
         <v>277</v>
@@ -4499,13 +4513,13 @@
         <v>210</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F80" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>278</v>
@@ -4531,13 +4545,13 @@
         <v>211</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F81" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>278</v>
@@ -4563,13 +4577,13 @@
         <v>212</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F82" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H82" s="8" t="s">
         <v>278</v>
@@ -4595,16 +4609,16 @@
         <v>208</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
@@ -4627,13 +4641,13 @@
         <v>209</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F84" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H84" s="8" t="s">
         <v>280</v>
@@ -4659,7 +4673,7 @@
         <v>214</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>204</v>
@@ -4691,13 +4705,13 @@
         <v>213</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H86" s="8" t="s">
         <v>277</v>
@@ -4723,13 +4737,13 @@
         <v>217</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H87" s="8" t="s">
         <v>278</v>
@@ -4755,13 +4769,13 @@
         <v>215</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>278</v>
@@ -4787,13 +4801,13 @@
         <v>216</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>282</v>
@@ -4819,23 +4833,23 @@
         <v>228</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I90" s="8"/>
       <c r="J90" s="15" t="s">
         <v>196</v>
       </c>
       <c r="K90" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="151.19999999999999" x14ac:dyDescent="0.3">
@@ -4853,13 +4867,13 @@
         <v>264</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H91" s="8" t="s">
         <v>283</v>
@@ -4885,7 +4899,7 @@
         <v>218</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F92" s="10" t="s">
         <v>204</v>
@@ -4917,7 +4931,7 @@
         <v>219</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F93" s="10" t="s">
         <v>204</v>
@@ -4951,7 +4965,7 @@
         <v>220</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>204</v>
@@ -4983,7 +4997,7 @@
         <v>221</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F95" s="10" t="s">
         <v>204</v>
@@ -5015,7 +5029,7 @@
         <v>222</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F96" s="10" t="s">
         <v>204</v>
@@ -5047,16 +5061,16 @@
         <v>223</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>297</v>
+        <v>384</v>
       </c>
       <c r="H97" s="12" t="s">
-        <v>327</v>
+        <v>383</v>
       </c>
       <c r="I97" s="8"/>
       <c r="J97" s="11" t="s">
@@ -5079,16 +5093,16 @@
         <v>224</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G98" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="H98" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="H98" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="I98" s="8"/>
       <c r="J98" s="11" t="s">
@@ -5111,7 +5125,7 @@
         <v>225</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F99" s="21" t="s">
         <v>204</v>
@@ -5123,7 +5137,7 @@
         <v>196</v>
       </c>
       <c r="K99" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="50.4" x14ac:dyDescent="0.3">
@@ -5141,7 +5155,7 @@
         <v>226</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F100" s="21" t="s">
         <v>204</v>
@@ -5171,7 +5185,7 @@
         <v>227</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F101" s="21" t="s">
         <v>204</v>
@@ -5201,7 +5215,7 @@
         <v>229</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F102" s="10" t="s">
         <v>204</v>
@@ -5210,7 +5224,7 @@
         <v>229</v>
       </c>
       <c r="H102" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I102" s="8"/>
       <c r="J102" s="11" t="s">
@@ -5233,7 +5247,7 @@
         <v>230</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F103" s="10" t="s">
         <v>204</v>
@@ -5265,13 +5279,13 @@
         <v>231</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H104" s="8" t="s">
         <v>277</v>
@@ -5297,13 +5311,13 @@
         <v>232</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F105" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H105" s="8" t="s">
         <v>278</v>
@@ -5329,13 +5343,13 @@
         <v>233</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F106" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H106" s="8" t="s">
         <v>278</v>
@@ -5361,13 +5375,13 @@
         <v>234</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F107" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H107" s="8" t="s">
         <v>278</v>
@@ -5393,16 +5407,16 @@
         <v>235</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F108" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I108" s="8"/>
       <c r="J108" s="11" t="s">
@@ -5422,26 +5436,26 @@
         <v>262</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F109" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H109" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I109" s="8"/>
       <c r="J109" s="15" t="s">
         <v>196</v>
       </c>
       <c r="K109" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="151.19999999999999" x14ac:dyDescent="0.3">
@@ -5456,26 +5470,26 @@
         <v>262</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F110" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I110" s="8"/>
       <c r="J110" s="15" t="s">
         <v>196</v>
       </c>
       <c r="K110" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="151.19999999999999" x14ac:dyDescent="0.3">
@@ -5490,16 +5504,16 @@
         <v>262</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F111" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H111" s="8" t="s">
         <v>280</v>
@@ -5525,7 +5539,7 @@
         <v>236</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F112" s="10" t="s">
         <v>204</v>
@@ -5534,7 +5548,7 @@
         <v>286</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I112" s="8"/>
       <c r="J112" s="11" t="s">
@@ -5557,13 +5571,13 @@
         <v>237</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F113" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G113" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>277</v>
@@ -5589,13 +5603,13 @@
         <v>238</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F114" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G114" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>278</v>
@@ -5621,13 +5635,13 @@
         <v>239</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F115" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G115" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>282</v>
@@ -5653,16 +5667,16 @@
         <v>265</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F116" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G116" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I116" s="8"/>
       <c r="J116" s="11" t="s">
@@ -5685,13 +5699,13 @@
         <v>266</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F117" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H117" s="8" t="s">
         <v>283</v>
@@ -5717,16 +5731,16 @@
         <v>240</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F118" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G118" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I118" s="8"/>
       <c r="J118" s="11" t="s">
@@ -5749,16 +5763,16 @@
         <v>267</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>279</v>
+        <v>381</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H119" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I119" s="8"/>
       <c r="J119" s="11" t="s">
@@ -5781,7 +5795,7 @@
         <v>268</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F120" s="10" t="s">
         <v>279</v>
@@ -5813,13 +5827,13 @@
         <v>241</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F121" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G121" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H121" s="12" t="s">
         <v>285</v>
@@ -5845,16 +5859,16 @@
         <v>242</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F122" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G122" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="H122" s="12" t="s">
         <v>319</v>
-      </c>
-      <c r="H122" s="12" t="s">
-        <v>320</v>
       </c>
       <c r="I122" s="8"/>
       <c r="J122" s="11" t="s">
@@ -5877,16 +5891,16 @@
         <v>269</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F123" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H123" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I123" s="8"/>
       <c r="J123" s="11" t="s">
@@ -5909,13 +5923,13 @@
         <v>270</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F124" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H124" s="8" t="s">
         <v>292</v>
@@ -5938,10 +5952,10 @@
         <v>262</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F125" s="10" t="s">
         <v>204</v>
@@ -5950,7 +5964,7 @@
         <v>293</v>
       </c>
       <c r="H125" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I125" s="8"/>
       <c r="J125" s="11" t="s">
@@ -5973,16 +5987,16 @@
         <v>244</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F126" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G126" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I126" s="8"/>
       <c r="J126" s="11" t="s">
@@ -6005,16 +6019,16 @@
         <v>245</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F127" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G127" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H127" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I127" s="8"/>
       <c r="J127" s="11" t="s">
@@ -6037,7 +6051,7 @@
         <v>243</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F128" s="21" t="s">
         <v>204</v>
@@ -6067,7 +6081,7 @@
         <v>246</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F129" s="21" t="s">
         <v>204</v>
@@ -6097,7 +6111,7 @@
         <v>247</v>
       </c>
       <c r="E130" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F130" s="21" t="s">
         <v>204</v>
@@ -6127,16 +6141,16 @@
         <v>248</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F131" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G131" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I131" s="8"/>
       <c r="J131" s="11" t="s">
@@ -6159,16 +6173,16 @@
         <v>249</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F132" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G132" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H132" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I132" s="8"/>
       <c r="J132" s="11" t="s">
@@ -6191,16 +6205,16 @@
         <v>250</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F133" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G133" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H133" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I133" s="8"/>
       <c r="J133" s="11" t="s">
@@ -6223,16 +6237,16 @@
         <v>251</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G134" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H134" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I134" s="8"/>
       <c r="J134" s="11" t="s">
@@ -6255,16 +6269,16 @@
         <v>252</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H135" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I135" s="8"/>
       <c r="J135" s="11" t="s">
@@ -6290,13 +6304,13 @@
         <v>274</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G136" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H136" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I136" s="8"/>
       <c r="J136" s="11" t="s">
@@ -6325,10 +6339,10 @@
         <v>199</v>
       </c>
       <c r="G137" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H137" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I137" s="8"/>
       <c r="J137" s="11" t="s">
@@ -6357,10 +6371,10 @@
         <v>199</v>
       </c>
       <c r="G138" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H138" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I138" s="8"/>
       <c r="J138" s="11" t="s">
@@ -6389,10 +6403,10 @@
         <v>199</v>
       </c>
       <c r="G139" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H139" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I139" s="8"/>
       <c r="J139" s="11" t="s">
@@ -6421,10 +6435,10 @@
         <v>199</v>
       </c>
       <c r="G140" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I140" s="8"/>
       <c r="J140" s="11" t="s">
@@ -6450,13 +6464,13 @@
         <v>202</v>
       </c>
       <c r="F141" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G141" s="9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H141" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I141" s="8"/>
       <c r="J141" s="11" t="s">
@@ -6482,13 +6496,13 @@
         <v>202</v>
       </c>
       <c r="F142" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G142" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H142" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I142" s="8"/>
       <c r="J142" s="11" t="s">
@@ -6511,16 +6525,16 @@
         <v>257</v>
       </c>
       <c r="E143" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G143" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H143" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I143" s="8"/>
       <c r="J143" s="11" t="s">
@@ -6549,10 +6563,10 @@
         <v>199</v>
       </c>
       <c r="G144" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H144" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I144" s="8"/>
       <c r="J144" s="11" t="s">
@@ -6581,10 +6595,10 @@
         <v>199</v>
       </c>
       <c r="G145" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H145" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I145" s="8"/>
       <c r="J145" s="11" t="s">
@@ -6613,10 +6627,10 @@
         <v>199</v>
       </c>
       <c r="G146" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H146" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I146" s="8"/>
       <c r="J146" s="11" t="s">
@@ -6645,10 +6659,10 @@
         <v>199</v>
       </c>
       <c r="G147" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I147" s="8"/>
       <c r="J147" s="11" t="s">

</xml_diff>